<commit_message>
0.2.12 - Finish PR calculations
</commit_message>
<xml_diff>
--- a/Source/Excel/TAF2_PR-205a/PR-205a_Load_Cases.xlsx
+++ b/Source/Excel/TAF2_PR-205a/PR-205a_Load_Cases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>*</t>
   </si>
@@ -95,19 +95,22 @@
     <t>Wind-Y Dynamic</t>
   </si>
   <si>
-    <t>Type=2  Mode=7  Normative ReliabilityFactor=1.4 21 6 10 1 3 0 0 2 95 6 1 0 0.3 2 0</t>
-  </si>
-  <si>
     <t>{"1":1,"3":0.95,"4":0.95,"5":0.95,"6":0.95, "9":0.5}</t>
   </si>
   <si>
-    <t>Type=2  Mode=42  Normative  LongTime=0.5  ReliabilityFactor=1.4</t>
-  </si>
-  <si>
     <t>Wind+Y Static</t>
   </si>
   <si>
     <t>Wind+Y Dynamic</t>
+  </si>
+  <si>
+    <t>Type=2  Mode=42  LongTime=0.5  ReliabilityFactor=1.4</t>
+  </si>
+  <si>
+    <t>Type=2  Mode=7  Normative ReliabilityFactor=1.4 21 20 10 1 3 0 0 2 95 6 1 0 0.3 2 0</t>
+  </si>
+  <si>
+    <t>Type=2  Mode=7  Normative ReliabilityFactor=1.4 21 20 11 1 3 0 0 2 95 6 1 0 0.3 2 0</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +631,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -636,7 +639,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>20</v>
@@ -667,13 +670,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -684,10 +687,10 @@
         <v>22</v>
       </c>
       <c r="C16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>